<commit_message>
Added scripts for monthly update and sales update
</commit_message>
<xml_diff>
--- a/Templates/Monthly/02 - February 2018 NL.xlsx
+++ b/Templates/Monthly/02 - February 2018 NL.xlsx
@@ -907,7 +907,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -918,7 +918,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>

</xml_diff>